<commit_message>
Fix InmemoryDB Primary Key's, Add SearchEngine and a couple of fixes in the header.
</commit_message>
<xml_diff>
--- a/Documents/InMemoryDB/InMemoryDBContentSeeder.xlsx
+++ b/Documents/InMemoryDB/InMemoryDBContentSeeder.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jelle\OneDrive\Haagse Hogeschool\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jelle\Documents\github\H2SE2a4_Project_Blok_6\Documents\InMemoryDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="373" documentId="8_{0521A16A-0D0A-46C9-A822-D3267A1AF429}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{E40888F4-469F-4EB8-9A61-2C73DC4DCD34}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D845186-838E-4EF6-9E5A-80FB6BF1A092}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6288" xr2:uid="{9A5A49E7-693B-471D-9EA4-4F9491F3F3CF}"/>
   </bookViews>
@@ -880,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1051FB7-A978-429A-9FCF-182322B73633}">
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -917,7 +917,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
@@ -928,7 +928,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
@@ -939,7 +939,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -961,7 +961,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
@@ -975,7 +975,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>6</v>
@@ -1000,7 +1000,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>8</v>
@@ -1014,7 +1014,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>9</v>
@@ -1028,7 +1028,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>10</v>
@@ -1042,7 +1042,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>11</v>
@@ -1064,7 +1064,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>13</v>
@@ -1075,7 +1075,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>14</v>
@@ -1086,7 +1086,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>16</v>
@@ -1114,7 +1114,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>5</v>
@@ -1134,7 +1134,7 @@
         <v>20</v>
       </c>
       <c r="B25" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>6</v>
@@ -1154,7 +1154,7 @@
         <v>21</v>
       </c>
       <c r="B26" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>6</v>
@@ -1188,7 +1188,7 @@
         <v>23</v>
       </c>
       <c r="B29" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>23</v>
@@ -1205,7 +1205,7 @@
         <v>24</v>
       </c>
       <c r="B30" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>24</v>
@@ -1222,7 +1222,7 @@
         <v>25</v>
       </c>
       <c r="B31" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>25</v>
@@ -1239,7 +1239,7 @@
         <v>26</v>
       </c>
       <c r="B32" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>26</v>
@@ -1267,7 +1267,7 @@
         <v>37</v>
       </c>
       <c r="B35" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>23</v>
@@ -1281,7 +1281,7 @@
         <v>38</v>
       </c>
       <c r="B36" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>26</v>
@@ -1295,7 +1295,7 @@
         <v>39</v>
       </c>
       <c r="B37" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>24</v>
@@ -1320,7 +1320,7 @@
         <v>42</v>
       </c>
       <c r="B40" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>25</v>
@@ -1334,7 +1334,7 @@
         <v>45</v>
       </c>
       <c r="B41" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>26</v>
@@ -1359,7 +1359,7 @@
         <v>47</v>
       </c>
       <c r="B44" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>65</v>
@@ -1373,7 +1373,7 @@
         <v>50</v>
       </c>
       <c r="B45" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>49</v>
@@ -1387,7 +1387,7 @@
         <v>51</v>
       </c>
       <c r="B46" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>52</v>
@@ -1401,7 +1401,7 @@
         <v>53</v>
       </c>
       <c r="B47" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>54</v>
@@ -1426,7 +1426,7 @@
         <v>56</v>
       </c>
       <c r="B50" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>26</v>
@@ -1440,7 +1440,7 @@
         <v>57</v>
       </c>
       <c r="B51" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>26</v>
@@ -1454,7 +1454,7 @@
         <v>58</v>
       </c>
       <c r="B52" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>23</v>
@@ -1479,7 +1479,7 @@
         <v>60</v>
       </c>
       <c r="B55" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>63</v>
@@ -1493,7 +1493,7 @@
         <v>61</v>
       </c>
       <c r="B56" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>14</v>
@@ -1507,7 +1507,7 @@
         <v>62</v>
       </c>
       <c r="B57" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>14</v>
@@ -1535,7 +1535,7 @@
         <v>67</v>
       </c>
       <c r="B60" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C60" s="4">
         <v>44137</v>
@@ -1552,7 +1552,7 @@
         <v>71</v>
       </c>
       <c r="B61" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C61" s="4">
         <v>44138</v>
@@ -1580,7 +1580,7 @@
         <v>73</v>
       </c>
       <c r="B64" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>67</v>
@@ -1594,7 +1594,7 @@
         <v>74</v>
       </c>
       <c r="B65" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>67</v>
@@ -1608,7 +1608,7 @@
         <v>75</v>
       </c>
       <c r="B66" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>71</v>
@@ -1633,7 +1633,7 @@
         <v>77</v>
       </c>
       <c r="B69" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>81</v>
@@ -1647,7 +1647,7 @@
         <v>78</v>
       </c>
       <c r="B70" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>82</v>
@@ -1661,7 +1661,7 @@
         <v>79</v>
       </c>
       <c r="B71" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>83</v>
@@ -1683,7 +1683,7 @@
         <v>87</v>
       </c>
       <c r="B74" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>87</v>
@@ -1694,7 +1694,7 @@
         <v>88</v>
       </c>
       <c r="B75" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>88</v>
@@ -1713,7 +1713,7 @@
         <v>96</v>
       </c>
       <c r="B78" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>92</v>
@@ -1724,7 +1724,7 @@
         <v>97</v>
       </c>
       <c r="B79" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>93</v>
@@ -1735,7 +1735,7 @@
         <v>95</v>
       </c>
       <c r="B80" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>94</v>
@@ -1757,7 +1757,7 @@
         <v>99</v>
       </c>
       <c r="B83" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>24</v>
@@ -1771,7 +1771,7 @@
         <v>100</v>
       </c>
       <c r="B84" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>25</v>
@@ -1785,7 +1785,7 @@
         <v>101</v>
       </c>
       <c r="B85" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>23</v>
@@ -1810,7 +1810,7 @@
         <v>103</v>
       </c>
       <c r="B88" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>13</v>
@@ -1824,7 +1824,7 @@
         <v>104</v>
       </c>
       <c r="B89" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>13</v>
@@ -1838,7 +1838,7 @@
         <v>105</v>
       </c>
       <c r="B90" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>14</v>
@@ -1852,7 +1852,7 @@
         <v>106</v>
       </c>
       <c r="B91" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>14</v>
@@ -1877,7 +1877,7 @@
         <v>108</v>
       </c>
       <c r="B94" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>96</v>
@@ -1891,7 +1891,7 @@
         <v>109</v>
       </c>
       <c r="B95" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>97</v>
@@ -1916,7 +1916,7 @@
         <v>112</v>
       </c>
       <c r="B98" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>112</v>
@@ -1930,7 +1930,7 @@
         <v>113</v>
       </c>
       <c r="B99" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>113</v>
@@ -1944,7 +1944,7 @@
         <v>114</v>
       </c>
       <c r="B100" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>114</v>
@@ -1969,7 +1969,7 @@
         <v>128</v>
       </c>
       <c r="B103" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>121</v>
@@ -1983,7 +1983,7 @@
         <v>124</v>
       </c>
       <c r="B104" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>122</v>
@@ -1997,7 +1997,7 @@
         <v>125</v>
       </c>
       <c r="B105" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>123</v>
@@ -2011,7 +2011,7 @@
         <v>126</v>
       </c>
       <c r="B106" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>127</v>
@@ -2036,7 +2036,7 @@
         <v>133</v>
       </c>
       <c r="B109" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>135</v>
@@ -2050,7 +2050,7 @@
         <v>132</v>
       </c>
       <c r="B110" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>136</v>
@@ -2072,7 +2072,7 @@
         <v>138</v>
       </c>
       <c r="B113" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>121</v>
@@ -2083,7 +2083,7 @@
         <v>139</v>
       </c>
       <c r="B114" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>140</v>

</xml_diff>

<commit_message>
Add more tests for the searchcontroller + Add WebsitePageID in Text and a couple of fixes in the InMemoryDB seeder.
</commit_message>
<xml_diff>
--- a/Documents/InMemoryDB/InMemoryDBContentSeeder.xlsx
+++ b/Documents/InMemoryDB/InMemoryDBContentSeeder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jelle\Documents\github\H2SE2a4_Project_Blok_6\Documents\InMemoryDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D845186-838E-4EF6-9E5A-80FB6BF1A092}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8CE5AC-EBB0-4FBC-8EA1-F53A93FCAFFC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6288" xr2:uid="{9A5A49E7-693B-471D-9EA4-4F9491F3F3CF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="150">
   <si>
     <t>Branch_Category</t>
   </si>
@@ -463,6 +463,24 @@
   </si>
   <si>
     <t>Percent</t>
+  </si>
+  <si>
+    <t>Profile_PhotoPath</t>
+  </si>
+  <si>
+    <t>/images/Henk.png</t>
+  </si>
+  <si>
+    <t>/images/Johan.png</t>
+  </si>
+  <si>
+    <t>/images/Marit.png</t>
+  </si>
+  <si>
+    <t>WebsitePageID</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -880,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1051FB7-A978-429A-9FCF-182322B73633}">
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1251,7 +1269,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B34" s="7" t="s">
         <v>36</v>
       </c>
@@ -1262,7 +1280,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
@@ -1276,7 +1294,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
@@ -1290,7 +1308,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
@@ -1304,7 +1322,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B39" s="7" t="s">
         <v>40</v>
       </c>
@@ -1315,7 +1333,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
@@ -1329,7 +1347,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
@@ -1343,7 +1361,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B43" s="7" t="s">
         <v>64</v>
       </c>
@@ -1353,8 +1371,11 @@
       <c r="D43" s="10" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E43" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>47</v>
       </c>
@@ -1367,8 +1388,11 @@
       <c r="D44" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>50</v>
       </c>
@@ -1381,8 +1405,11 @@
       <c r="D45" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
@@ -1395,8 +1422,11 @@
       <c r="D46" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E46" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>53</v>
       </c>
@@ -1408,6 +1438,9 @@
       </c>
       <c r="D47" s="2" t="s">
         <v>78</v>
+      </c>
+      <c r="E47" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1900,7 +1933,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B97" s="7" t="s">
         <v>111</v>
       </c>
@@ -1910,8 +1943,11 @@
       <c r="D97" s="10" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E97" s="10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>112</v>
       </c>
@@ -1924,8 +1960,11 @@
       <c r="D98" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E98" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>113</v>
       </c>
@@ -1938,8 +1977,11 @@
       <c r="D99" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E99" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>114</v>
       </c>
@@ -1952,8 +1994,11 @@
       <c r="D100" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E100" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B102" s="7" t="s">
         <v>119</v>
       </c>
@@ -1964,7 +2009,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>128</v>
       </c>
@@ -1978,7 +2023,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>124</v>
       </c>
@@ -1992,7 +2037,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>125</v>
       </c>
@@ -2006,7 +2051,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>126</v>
       </c>
@@ -2020,7 +2065,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B108" s="7" t="s">
         <v>129</v>
       </c>
@@ -2031,7 +2076,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>133</v>
       </c>
@@ -2045,7 +2090,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>132</v>
       </c>
@@ -2059,7 +2104,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B112" s="7" t="s">
         <v>137</v>
       </c>

</xml_diff>